<commit_message>
Cube ok. number voice.
</commit_message>
<xml_diff>
--- a/rubik.02.xlsx
+++ b/rubik.02.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="152">
   <si>
     <t>center=</t>
   </si>
@@ -239,22 +239,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1(F)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>4(L)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5(R)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>3(B)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>2(D)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -468,6 +452,149 @@
   </si>
   <si>
     <t>B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>11()2</t>
+  </si>
+  <si>
+    <t>14(RD)5</t>
+  </si>
+  <si>
+    <t>17()8</t>
+  </si>
+  <si>
+    <t>10(RB)1</t>
+  </si>
+  <si>
+    <t>16(RF)7</t>
+  </si>
+  <si>
+    <t>9(rub)0</t>
+  </si>
+  <si>
+    <t>12(RU)3</t>
+  </si>
+  <si>
+    <t>15()6</t>
+  </si>
+  <si>
+    <t>47()2</t>
+  </si>
+  <si>
+    <t>50(BR)5</t>
+  </si>
+  <si>
+    <t>53()8</t>
+  </si>
+  <si>
+    <t>38()2</t>
+  </si>
+  <si>
+    <t>41(FR)5</t>
+  </si>
+  <si>
+    <t>44()8</t>
+  </si>
+  <si>
+    <t>21(dr)3</t>
+  </si>
+  <si>
+    <t>18(dbr)0</t>
+  </si>
+  <si>
+    <t>46(BD)1</t>
+  </si>
+  <si>
+    <t>37(FU)1</t>
+  </si>
+  <si>
+    <t>43(fd)7</t>
+  </si>
+  <si>
+    <t>19(db)1</t>
+  </si>
+  <si>
+    <t>45()0</t>
+  </si>
+  <si>
+    <t>51()6</t>
+  </si>
+  <si>
+    <t>36()0</t>
+  </si>
+  <si>
+    <t>39(FL)3</t>
+  </si>
+  <si>
+    <t>42()6</t>
+  </si>
+  <si>
+    <t>23(dl)5</t>
+  </si>
+  <si>
+    <t>20(dlb)2</t>
+  </si>
+  <si>
+    <t>29()2</t>
+  </si>
+  <si>
+    <t>35()8</t>
+  </si>
+  <si>
+    <t>28(LB)1</t>
+  </si>
+  <si>
+    <t>27()0</t>
+  </si>
+  <si>
+    <t>30(LD)3</t>
+  </si>
+  <si>
+    <t>33()6</t>
+  </si>
+  <si>
+    <t>4(F)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1(R)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3(L)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5(B)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1(R)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(F)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5(B)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52(BU)7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>32(LU)5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>34(LF)7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>48(BL)3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1491,7 +1618,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6016,16 +6143,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
@@ -6066,7 +6193,7 @@
         <v>9</v>
       </c>
       <c r="M2">
-        <f>C2*10+E2</f>
+        <f t="shared" ref="M2:M33" si="0">C2*10+E2</f>
         <v>54</v>
       </c>
       <c r="N2">
@@ -6111,7 +6238,7 @@
         <v>9</v>
       </c>
       <c r="M3">
-        <f>C3*10+E3</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="N3">
@@ -6156,7 +6283,7 @@
         <v>9</v>
       </c>
       <c r="M4">
-        <f>C4*10+E4</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="N4">
@@ -6201,7 +6328,7 @@
         <v>9</v>
       </c>
       <c r="M5">
-        <f>C5*10+E5</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="N5">
@@ -6246,7 +6373,7 @@
         <v>12</v>
       </c>
       <c r="M6">
-        <f>C6*10+E6</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="N6">
@@ -6291,7 +6418,7 @@
         <v>12</v>
       </c>
       <c r="M7">
-        <f>C7*10+E7</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="N7">
@@ -6336,7 +6463,7 @@
         <v>12</v>
       </c>
       <c r="M8">
-        <f>C8*10+E8</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="N8">
@@ -6381,7 +6508,7 @@
         <v>9</v>
       </c>
       <c r="M9">
-        <f>C9*10+E9</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="N9">
@@ -6426,7 +6553,7 @@
         <v>9</v>
       </c>
       <c r="M10">
-        <f>C10*10+E10</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="N10">
@@ -6471,7 +6598,7 @@
         <v>13</v>
       </c>
       <c r="M11">
-        <f>C11*10+E11</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="N11">
@@ -6516,7 +6643,7 @@
         <v>13</v>
       </c>
       <c r="M12">
-        <f>C12*10+E12</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="N12">
@@ -6561,7 +6688,7 @@
         <v>13</v>
       </c>
       <c r="M13">
-        <f>C13*10+E13</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="N13">
@@ -6606,7 +6733,7 @@
         <v>13</v>
       </c>
       <c r="M14">
-        <f>C14*10+E14</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="N14">
@@ -6651,7 +6778,7 @@
         <v>13</v>
       </c>
       <c r="M15">
-        <f>C15*10+E15</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N15">
@@ -6696,7 +6823,7 @@
         <v>13</v>
       </c>
       <c r="M16">
-        <f>C16*10+E16</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="N16">
@@ -6741,7 +6868,7 @@
         <v>13</v>
       </c>
       <c r="M17">
-        <f>C17*10+E17</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="N17">
@@ -6786,7 +6913,7 @@
         <v>13</v>
       </c>
       <c r="M18">
-        <f>C18*10+E18</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="N18">
@@ -6831,7 +6958,7 @@
         <v>13</v>
       </c>
       <c r="M19">
-        <f>C19*10+E19</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="N19">
@@ -6876,7 +7003,7 @@
         <v>16</v>
       </c>
       <c r="M20">
-        <f>C20*10+E20</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="N20">
@@ -6921,7 +7048,7 @@
         <v>17</v>
       </c>
       <c r="M21">
-        <f>C21*10+E21</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="N21">
@@ -6966,7 +7093,7 @@
         <v>17</v>
       </c>
       <c r="M22">
-        <f>C22*10+E22</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="N22">
@@ -7011,7 +7138,7 @@
         <v>16</v>
       </c>
       <c r="M23">
-        <f>C23*10+E23</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="N23">
@@ -7056,7 +7183,7 @@
         <v>16</v>
       </c>
       <c r="M24">
-        <f>C24*10+E24</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="N24">
@@ -7101,7 +7228,7 @@
         <v>16</v>
       </c>
       <c r="M25">
-        <f>C25*10+E25</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="N25">
@@ -7146,7 +7273,7 @@
         <v>16</v>
       </c>
       <c r="M26">
-        <f>C26*10+E26</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="N26">
@@ -7191,7 +7318,7 @@
         <v>16</v>
       </c>
       <c r="M27">
-        <f>C27*10+E27</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="N27">
@@ -7236,7 +7363,7 @@
         <v>17</v>
       </c>
       <c r="M28">
-        <f>C28*10+E28</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="N28">
@@ -7281,7 +7408,7 @@
         <v>19</v>
       </c>
       <c r="M29">
-        <f>C29*10+E29</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="N29">
@@ -7326,7 +7453,7 @@
         <v>19</v>
       </c>
       <c r="M30">
-        <f>C30*10+E30</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="N30">
@@ -7371,7 +7498,7 @@
         <v>19</v>
       </c>
       <c r="M31">
-        <f>C31*10+E31</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="N31">
@@ -7416,7 +7543,7 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <f>C32*10+E32</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="N32">
@@ -7461,7 +7588,7 @@
         <v>19</v>
       </c>
       <c r="M33">
-        <f>C33*10+E33</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="N33">
@@ -7506,7 +7633,7 @@
         <v>19</v>
       </c>
       <c r="M34">
-        <f>C34*10+E34</f>
+        <f t="shared" ref="M34:M55" si="1">C34*10+E34</f>
         <v>33</v>
       </c>
       <c r="N34">
@@ -7551,7 +7678,7 @@
         <v>19</v>
       </c>
       <c r="M35">
-        <f>C35*10+E35</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="N35">
@@ -7596,7 +7723,7 @@
         <v>19</v>
       </c>
       <c r="M36">
-        <f>C36*10+E36</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="N36">
@@ -7641,7 +7768,7 @@
         <v>19</v>
       </c>
       <c r="M37">
-        <f>C37*10+E37</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="N37">
@@ -7686,7 +7813,7 @@
         <v>12</v>
       </c>
       <c r="M38">
-        <f>C38*10+E38</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="N38">
@@ -7731,7 +7858,7 @@
         <v>12</v>
       </c>
       <c r="M39">
-        <f>C39*10+E39</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="N39">
@@ -7776,7 +7903,7 @@
         <v>12</v>
       </c>
       <c r="M40">
-        <f>C40*10+E40</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="N40">
@@ -7821,7 +7948,7 @@
         <v>12</v>
       </c>
       <c r="M41">
-        <f>C41*10+E41</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="N41">
@@ -7866,7 +7993,7 @@
         <v>16</v>
       </c>
       <c r="M42">
-        <f>C42*10+E42</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="N42">
@@ -7911,7 +8038,7 @@
         <v>16</v>
       </c>
       <c r="M43">
-        <f>C43*10+E43</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="N43">
@@ -7956,7 +8083,7 @@
         <v>16</v>
       </c>
       <c r="M44">
-        <f>C44*10+E44</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="N44">
@@ -8001,7 +8128,7 @@
         <v>12</v>
       </c>
       <c r="M45">
-        <f>C45*10+E45</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="N45">
@@ -8046,7 +8173,7 @@
         <v>12</v>
       </c>
       <c r="M46">
-        <f>C46*10+E46</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="N46">
@@ -8091,7 +8218,7 @@
         <v>17</v>
       </c>
       <c r="M47">
-        <f>C47*10+E47</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="N47">
@@ -8136,7 +8263,7 @@
         <v>9</v>
       </c>
       <c r="M48">
-        <f>C48*10+E48</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N48">
@@ -8181,7 +8308,7 @@
         <v>9</v>
       </c>
       <c r="M49">
-        <f>C49*10+E49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N49">
@@ -8226,7 +8353,7 @@
         <v>17</v>
       </c>
       <c r="M50">
-        <f>C50*10+E50</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N50">
@@ -8271,7 +8398,7 @@
         <v>17</v>
       </c>
       <c r="M51">
-        <f>C51*10+E51</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N51">
@@ -8316,7 +8443,7 @@
         <v>17</v>
       </c>
       <c r="M52">
-        <f>C52*10+E52</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="N52">
@@ -8361,7 +8488,7 @@
         <v>17</v>
       </c>
       <c r="M53">
-        <f>C53*10+E53</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="N53">
@@ -8406,7 +8533,7 @@
         <v>17</v>
       </c>
       <c r="M54">
-        <f>C54*10+E54</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="N54">
@@ -8451,7 +8578,7 @@
         <v>22</v>
       </c>
       <c r="M55">
-        <f>C55*10+E55</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N55">
@@ -8472,228 +8599,415 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:12" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:22" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="D2" s="45" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D3" s="48" t="s">
-        <v>76</v>
+        <v>151</v>
       </c>
       <c r="E3" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="F3" s="49" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" s="5" t="s">
+      <c r="E7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" s="8" t="s">
+      <c r="K7" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L7" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D8" s="27" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D9" s="30" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>55</v>
+        <v>141</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D10" s="33" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="S15" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="T15" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="U15" s="47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="T16" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="U16" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="V16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="S17" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="T17" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="U17" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>0</v>
+      </c>
+      <c r="P18" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q18" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="R18" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V18" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="W18" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="X18" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="P19" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q19" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="R19" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="T19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="U19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="V19" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="W19" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="X19" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="P20" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q20" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="R20" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="T20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="V20" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="W20" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="X20" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA20" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="S21" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="T21" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="U21" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="R22">
+        <v>3</v>
+      </c>
+      <c r="S22" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="T22" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="U22" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="S23" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="T23" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="U23" s="35" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>